<commit_message>
tweede iteratie gedaan, derde staat klaar
</commit_message>
<xml_diff>
--- a/Identifier/Old to label/Iterations.xlsx
+++ b/Identifier/Old to label/Iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefva\Documents\Master\Thesis_s2\Code\Identifier\Old to label\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDAABD3-5FEE-4241-8B1E-4D3DA0161C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D672CA03-AC89-4086-8992-D11BF617B5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">iteration </t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>61/200</t>
+  </si>
+  <si>
+    <t>69/200</t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,6 +378,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
derde iterarie gedaan van de identifier, vierde staat klaar
</commit_message>
<xml_diff>
--- a/Identifier/Old to label/Iterations.xlsx
+++ b/Identifier/Old to label/Iterations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefva\Documents\Master\Thesis_s2\Code\Identifier\Old to label\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D672CA03-AC89-4086-8992-D11BF617B5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3596C008-C6BE-41F7-917A-F4EF3704AE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">iteration </t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>69/200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">training data </t>
+  </si>
+  <si>
+    <t>32/200</t>
   </si>
 </sst>
 </file>
@@ -354,36 +360,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vijfde iteratie gedaan, zesde staat klaar
</commit_message>
<xml_diff>
--- a/Identifier/Old to label/Iterations.xlsx
+++ b/Identifier/Old to label/Iterations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefva\Documents\Master\Thesis_s2\Code\Identifier\Old to label\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3596C008-C6BE-41F7-917A-F4EF3704AE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB344094-85E5-4C00-91E6-B4192AE64133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">iteration </t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>32/200</t>
+  </si>
+  <si>
+    <t>41/200</t>
+  </si>
+  <si>
+    <t>44/200</t>
   </si>
 </sst>
 </file>
@@ -360,15 +366,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,7 +385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -390,7 +396,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -401,7 +407,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -410,6 +416,28 @@
       </c>
       <c r="C4">
         <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>1600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
zesde iteratie gedaan, zevende staat klaar
</commit_message>
<xml_diff>
--- a/Identifier/Old to label/Iterations.xlsx
+++ b/Identifier/Old to label/Iterations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefva\Documents\Master\Thesis_s2\Code\Identifier\Old to label\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB344094-85E5-4C00-91E6-B4192AE64133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E21AAD-5F8D-4DE1-8E73-FF4366EC8DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">iteration </t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>44/200</t>
+  </si>
+  <si>
+    <t>56/200</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,6 +443,17 @@
         <v>1600</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1800</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
zevende iteratie gedaan, achtste staat klaar
</commit_message>
<xml_diff>
--- a/Identifier/Old to label/Iterations.xlsx
+++ b/Identifier/Old to label/Iterations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefva\Documents\Master\Thesis_s2\Code\Identifier\Old to label\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E21AAD-5F8D-4DE1-8E73-FF4366EC8DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D700AA6E-2B30-4591-AD2D-D8E1A1075186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">iteration </t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>56/200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45/200 </t>
   </si>
 </sst>
 </file>
@@ -369,15 +372,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,7 +391,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -399,7 +402,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -410,7 +413,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -421,7 +424,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -432,7 +435,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -443,7 +446,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -452,6 +455,17 @@
       </c>
       <c r="C7">
         <v>1800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
paar mberts geprobeerd, alsook de identifier opgesplits in breed en eng, achtste iteratie gedaan negende staat klaar
</commit_message>
<xml_diff>
--- a/Identifier/Old to label/Iterations.xlsx
+++ b/Identifier/Old to label/Iterations.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefva\Documents\Master\Thesis_s2\Code\Identifier\Old to label\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D700AA6E-2B30-4591-AD2D-D8E1A1075186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88879D4-02DC-40A8-BBDC-92797266D9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">iteration </t>
   </si>
@@ -55,6 +66,18 @@
   </si>
   <si>
     <t xml:space="preserve">45/200 </t>
+  </si>
+  <si>
+    <t>33/200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iteration </t>
+  </si>
+  <si>
+    <t>difference</t>
+  </si>
+  <si>
+    <t>TP</t>
   </si>
 </sst>
 </file>
@@ -372,15 +395,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,8 +413,20 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -401,8 +436,20 @@
       <c r="C2">
         <v>500</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -413,7 +460,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -424,7 +471,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -435,7 +482,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -446,7 +493,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -457,7 +504,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -466,6 +513,17 @@
       </c>
       <c r="C8">
         <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>2200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>